<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@3eccf2017a58f77d3b0613215df1dc40f0980b2f 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-patient.xlsx
+++ b/StructureDefinition-us-core-patient.xlsx
@@ -343,7 +343,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) US Core Race Extension</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: US Core Race Extension</t>
   </si>
   <si>
     <t>Concepts classifying the person into a named category of humans sharing common history, traits, geographical origin or nationality.  The race codes used to represent these concepts are based upon the [CDC Race and Ethnicity Code Set Version 1.0](http://www.cdc.gov/phin/resources/vocabulary/index.html) which includes over 900 concepts for representing race and ethnicity of which 921 reference race.  The race concepts are grouped by and pre-mapped to the 5 OMB race categories:
@@ -368,7 +368,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) US Core ethnicity Extension</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: US Core ethnicity Extension</t>
   </si>
   <si>
     <t>Concepts classifying the person into a named category of humans sharing common history, traits, geographical origin or nationality.  The ethnicity codes used to represent these concepts are based upon the [CDC ethnicity and Ethnicity Code Set Version 1.0](http://www.cdc.gov/phin/resources/vocabulary/index.html) which includes over 900 concepts for representing race and ethnicity of which 43 reference ethnicity.  The ethnicity concepts are grouped by and pre-mapped to the 2 OMB ethnicity categories: - Hispanic or Latino - Not Hispanic or Latino.</t>
@@ -384,7 +384,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) Tribal Affiliation Extension</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: Tribal Affiliation Extension</t>
   </si>
   <si>
     <t>A tribe or band with which a person associates whether or not they are an enrolled member.</t>
@@ -422,7 +422,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) Sex Extension</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: Sex Extension</t>
   </si>
   <si>
     <t>The US Core Sex Extension is used to reflect the documentation of a person's sex. It aligns with the C-CDA Sex Observation (LOINC 46098-0).</t>
@@ -438,7 +438,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) The individual's gender identity</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: The individual's gender identity</t>
   </si>
   <si>
     <t>An individual's personal sense of being a man, woman, boy, girl, nonbinary, or something else.</t>
@@ -766,7 +766,7 @@
     <t>Patient.name.use</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) usual | official | temp | nickname | anonymous | old | maiden</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: usual | official | temp | nickname | anonymous | old | maiden</t>
   </si>
   <si>
     <t>Identifies the purpose for this name.</t>
@@ -910,7 +910,7 @@
     <t>Patient.name.period</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) Time period when name was/is in use</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: Time period when name was/is in use</t>
   </si>
   <si>
     <t>Indicates the period of time when this name was valid for the named person.</t>
@@ -935,7 +935,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) A contact detail for the individual</t>
+    <t>A contact detail for the individual</t>
   </si>
   <si>
     <t>A contact detail (e.g. a telephone number or an email address) by which the individual may be contacted.</t>
@@ -1131,7 +1131,7 @@
 dateTime</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) Indicates if the individual is deceased or not</t>
+    <t>Indicates if the individual is deceased or not</t>
   </si>
   <si>
     <t>Indicates if the individual is deceased or not.</t>
@@ -1186,7 +1186,7 @@
     <t>Patient.address.use</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) home | work | temp | old | billing - purpose of this address</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: home | work | temp | old | billing - purpose of this address</t>
   </si>
   <si>
     <t>The purpose of this address.</t>
@@ -1412,7 +1412,7 @@
     <t>Patient.address.period</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) Time period when address was/is in use</t>
+    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: Time period when address was/is in use</t>
   </si>
   <si>
     <t>Time period when address was/is in use.</t>
@@ -1686,7 +1686,7 @@
     <t>Patient.communication</t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: ❗(𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜) A language which may be used to communicate with the patient about his or her health</t>
+    <t>A language which may be used to communicate with the patient about his or her health</t>
   </si>
   <si>
     <t>A language which may be used to communicate with the patient about his or her health.</t>

</xml_diff>